<commit_message>
Update schematics to rev 1.2
</commit_message>
<xml_diff>
--- a/Hardware/PCB/BOM_KorreKthor.xlsx
+++ b/Hardware/PCB/BOM_KorreKthor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\École\ECAM - 1ère Master\Robotic Project\KorreKthor\Hardware\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{139B89E9-B3DC-452B-BED8-A97FF78F4CC6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B72C9EEC-6C45-4890-9FBC-0A0598CC136A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="BOM_KorreKthor" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="BOM_KorreKthor" localSheetId="0">BOM_KorreKthor!$A$20:$F$38</definedName>
     <definedName name="BOM_KorreKthor_1" localSheetId="0">BOM_KorreKthor!$A$1:$F$17</definedName>
   </definedNames>
   <calcPr calcId="0"/>
@@ -36,11 +37,23 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="2" xr16:uid="{2A0B878F-49AE-431B-9815-7BB56DD023B5}" name="BOM_KorreKthor1" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="850" sourceFile="E:\Documents\École\ECAM - 1ère Master\Robotic Project\KorreKthor\Hardware\PCB\KorreKthor\Project Outputs for KorreKthor\BOM_KorreKthor.csv" decimal="," thousands="." comma="1">
+      <textFields count="6">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="67">
   <si>
     <t>Comment</t>
   </si>
@@ -99,18 +112,9 @@
     <t>LED RGB</t>
   </si>
   <si>
-    <t>Relay-SPDT</t>
-  </si>
-  <si>
-    <t>Single-Pole Dual-Throw Relay</t>
-  </si>
-  <si>
     <t>K1, K2</t>
   </si>
   <si>
-    <t>MODULE5B</t>
-  </si>
-  <si>
     <t>Buzzer</t>
   </si>
   <si>
@@ -126,15 +130,9 @@
     <t>Header, 3-Pin</t>
   </si>
   <si>
-    <t>HDR1X3</t>
-  </si>
-  <si>
     <t>Header, 2-Pin</t>
   </si>
   <si>
-    <t>HDR1X2</t>
-  </si>
-  <si>
     <t>Rasberry Pi Connector</t>
   </si>
   <si>
@@ -150,9 +148,6 @@
     <t>Header, 11-Pin</t>
   </si>
   <si>
-    <t>HDR1X11</t>
-  </si>
-  <si>
     <t>2N2222</t>
   </si>
   <si>
@@ -232,6 +227,33 @@
   </si>
   <si>
     <t>https://be.farnell.com/fr-BE/wurth-elektronik/61304021821/connect-femelle-40-voies-2-rangs/dp/2827916</t>
+  </si>
+  <si>
+    <t>Relay-SPST</t>
+  </si>
+  <si>
+    <t>Single-Pole Single-Throw Relay</t>
+  </si>
+  <si>
+    <t>MODULE4</t>
+  </si>
+  <si>
+    <t>Conn_1X3</t>
+  </si>
+  <si>
+    <t>Bornier_1X2</t>
+  </si>
+  <si>
+    <t>Conn_1X11</t>
+  </si>
+  <si>
+    <t>HW-411_Buck_converter</t>
+  </si>
+  <si>
+    <t>Buck converter board</t>
+  </si>
+  <si>
+    <t>U1</t>
   </si>
 </sst>
 </file>
@@ -785,6 +807,10 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="BOM_KorreKthor" connectionId="2" xr16:uid="{CB3BB0C0-A179-4C15-A48E-2256DCF0B7DF}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="BOM_KorreKthor_1" connectionId="1" xr16:uid="{A5F9B11C-8F24-4631-BFCA-B64F455D16BA}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
@@ -1085,10 +1111,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1097,7 +1123,7 @@
     <col min="2" max="2" width="30.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="107" customWidth="1"/>
   </cols>
@@ -1113,7 +1139,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -1122,7 +1148,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1142,7 +1168,7 @@
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1162,7 +1188,7 @@
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1182,7 +1208,7 @@
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1202,236 +1228,256 @@
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" t="s">
         <v>19</v>
       </c>
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" t="s">
-        <v>21</v>
-      </c>
       <c r="E7" t="s">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="F7">
         <v>2</v>
       </c>
       <c r="G7" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" t="s">
         <v>23</v>
-      </c>
-      <c r="B8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" t="s">
-        <v>26</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E9" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="F9">
         <v>3</v>
       </c>
       <c r="G9" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E10" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="F10">
         <v>3</v>
       </c>
       <c r="G10" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E11" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="F11">
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E12" t="s">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="F12">
         <v>2</v>
       </c>
       <c r="G12" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E13" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F13">
         <v>2</v>
       </c>
       <c r="G13" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D14" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="E14" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="F14">
         <v>2</v>
       </c>
       <c r="G14" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C15" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D15" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E15" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="F15">
         <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D16">
         <v>100</v>
       </c>
       <c r="E16" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="F16">
         <v>4</v>
       </c>
       <c r="G16" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C17" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E17" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F17">
         <v>4</v>
       </c>
       <c r="G17" t="s">
-        <v>47</v>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update schematics to rev 1.3
</commit_message>
<xml_diff>
--- a/Hardware/PCB/BOM_KorreKthor.xlsx
+++ b/Hardware/PCB/BOM_KorreKthor.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\École\ECAM - 1ère Master\Robotic Project\KorreKthor\Hardware\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B72C9EEC-6C45-4890-9FBC-0A0598CC136A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{207250E8-0FBF-4000-8A6F-7BEF7BB17D26}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_KorreKthor" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="BOM_KorreKthor" localSheetId="0">BOM_KorreKthor!$A$20:$F$38</definedName>
-    <definedName name="BOM_KorreKthor_1" localSheetId="0">BOM_KorreKthor!$A$1:$F$17</definedName>
+    <definedName name="BOM_KorreKthor" localSheetId="0">BOM_KorreKthor!$A$21:$F$38</definedName>
+    <definedName name="BOM_KorreKthor_1" localSheetId="0">BOM_KorreKthor!$A$1:$F$19</definedName>
+    <definedName name="BOM_KorreKthor_2" localSheetId="0">BOM_KorreKthor!$A$21:$F$38</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -49,11 +50,23 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="3" xr16:uid="{650365C4-9443-4D36-A91F-B3E4A4E1E62F}" name="BOM_KorreKthor2" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="850" sourceFile="E:\Documents\École\ECAM - 1ère Master\Robotic Project\KorreKthor\Hardware\PCB\KorreKthor\Project Outputs for KorreKthor\BOM_KorreKthor.csv" decimal="," thousands="." tab="0" comma="1">
+      <textFields count="6">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="76">
   <si>
     <t>Comment</t>
   </si>
@@ -82,9 +95,6 @@
     <t>DO-41</t>
   </si>
   <si>
-    <t>ON</t>
-  </si>
-  <si>
     <t>Typical INFRARED GaAs LED</t>
   </si>
   <si>
@@ -124,9 +134,6 @@
     <t>LS1</t>
   </si>
   <si>
-    <t>ABSM-1574</t>
-  </si>
-  <si>
     <t>Header, 3-Pin</t>
   </si>
   <si>
@@ -142,9 +149,6 @@
     <t>P7</t>
   </si>
   <si>
-    <t>MHDR2X20</t>
-  </si>
-  <si>
     <t>Header, 11-Pin</t>
   </si>
   <si>
@@ -172,9 +176,6 @@
     <t>Switch</t>
   </si>
   <si>
-    <t>SPST-2</t>
-  </si>
-  <si>
     <t>Link</t>
   </si>
   <si>
@@ -235,9 +236,6 @@
     <t>Single-Pole Single-Throw Relay</t>
   </si>
   <si>
-    <t>MODULE4</t>
-  </si>
-  <si>
     <t>Conn_1X3</t>
   </si>
   <si>
@@ -254,6 +252,48 @@
   </si>
   <si>
     <t>U1</t>
+  </si>
+  <si>
+    <t>Cap Pol1</t>
+  </si>
+  <si>
+    <t>Polarized Capacitor (Radial)</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>10u</t>
+  </si>
+  <si>
+    <t>Rad5.2</t>
+  </si>
+  <si>
+    <t>Cap</t>
+  </si>
+  <si>
+    <t>Capacitor</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>100n</t>
+  </si>
+  <si>
+    <t>RAD-0.2</t>
+  </si>
+  <si>
+    <t>Power</t>
+  </si>
+  <si>
+    <t>RELAY_OJE-SH_series</t>
+  </si>
+  <si>
+    <t>HDR2X20</t>
+  </si>
+  <si>
+    <t>SW_1825910-6-4</t>
   </si>
 </sst>
 </file>
@@ -807,11 +847,15 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="BOM_KorreKthor" connectionId="2" xr16:uid="{CB3BB0C0-A179-4C15-A48E-2256DCF0B7DF}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="BOM_KorreKthor_2" connectionId="3" xr16:uid="{3626DFE5-37EE-457C-85AD-85542F52254E}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="BOM_KorreKthor_1" connectionId="1" xr16:uid="{A5F9B11C-8F24-4631-BFCA-B64F455D16BA}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="BOM_KorreKthor" connectionId="2" xr16:uid="{CB3BB0C0-A179-4C15-A48E-2256DCF0B7DF}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1111,10 +1155,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1139,7 +1183,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -1148,336 +1192,382 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>63</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>64</v>
+      </c>
+      <c r="D3" t="s">
+        <v>65</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="F3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>67</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>69</v>
+      </c>
+      <c r="D4" t="s">
+        <v>70</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>71</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>72</v>
       </c>
       <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E7" t="s">
-        <v>60</v>
+        <v>14</v>
       </c>
       <c r="F7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>55</v>
       </c>
       <c r="C9" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="E9" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="F9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G9" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="E10" t="s">
-        <v>62</v>
+        <v>19</v>
       </c>
       <c r="F10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="E11" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G11" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E12" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G12" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E13" t="s">
-        <v>34</v>
+        <v>74</v>
       </c>
       <c r="F13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>49</v>
-      </c>
-      <c r="D14" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E14" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="F14">
         <v>2</v>
       </c>
       <c r="G14" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="E15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+      <c r="G15" t="s">
         <v>37</v>
-      </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-      <c r="G15" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
-      </c>
-      <c r="D16">
-        <v>100</v>
+        <v>45</v>
+      </c>
+      <c r="D16" t="s">
+        <v>46</v>
       </c>
       <c r="E16" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16">
+        <v>2</v>
+      </c>
+      <c r="G16" t="s">
         <v>37</v>
-      </c>
-      <c r="F16">
-        <v>4</v>
-      </c>
-      <c r="G16" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
+        <v>47</v>
+      </c>
+      <c r="D17" t="s">
+        <v>48</v>
       </c>
       <c r="E17" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F17">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="B18" t="s">
-        <v>65</v>
+        <v>33</v>
       </c>
       <c r="C18" t="s">
-        <v>66</v>
+        <v>49</v>
+      </c>
+      <c r="D18">
+        <v>100</v>
       </c>
       <c r="E18" t="s">
-        <v>64</v>
+        <v>34</v>
       </c>
       <c r="F18">
+        <v>4</v>
+      </c>
+      <c r="G18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19" t="s">
+        <v>75</v>
+      </c>
+      <c r="F19">
+        <v>4</v>
+      </c>
+      <c r="G19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20" t="s">
+        <v>59</v>
+      </c>
+      <c r="F20">
         <v>1</v>
       </c>
-      <c r="G18" t="s">
-        <v>41</v>
+      <c r="G20" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>